<commit_message>
Week 5 Tutorial project added, small changes to week 4 spreadsheet
</commit_message>
<xml_diff>
--- a/Week4/KIT205_Week3.xlsx
+++ b/Week4/KIT205_Week3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/bronsonb_utas_edu_au/Documents/2025 - S1/KIT205/KIT205_575952/Week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="11_F7D9FA504A20DB2F5DD148760D251FD299863421" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C79FFA5-53B0-4235-B405-7B07E7D17B50}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="11_F7D9FA504A20DB2F5DD148760D251FD299863421" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4173CE1C-E306-4772-8C6C-CA244C66B0CD}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="683" windowWidth="14400" windowHeight="8182" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,6 +202,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,16 +473,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="9" max="11" width="14.7109375" customWidth="1"/>
+    <col min="9" max="11" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
@@ -489,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="I3" s="3">
         <v>1</v>
       </c>
@@ -500,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -576,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f>A5*2</f>
         <v>2</v>
@@ -615,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -653,7 +657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A26" si="3">A7*2</f>
         <v>10</v>
@@ -692,7 +696,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -731,7 +735,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>50</v>
       </c>
@@ -769,7 +773,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -808,7 +812,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="3"/>
         <v>200</v>
@@ -847,7 +851,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>500</v>
       </c>
@@ -885,7 +889,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="3"/>
         <v>1000</v>
@@ -922,7 +926,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="3"/>
         <v>2000</v>
@@ -959,7 +963,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>5000</v>
       </c>
@@ -995,7 +999,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="3"/>
         <v>10000</v>
@@ -1032,7 +1036,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="3"/>
         <v>20000</v>
@@ -1069,7 +1073,7 @@
         <v>400000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>50000</v>
       </c>
@@ -1105,7 +1109,7 @@
         <v>2500000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="3"/>
         <v>100000</v>
@@ -1140,7 +1144,7 @@
         <v>10000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="3"/>
         <v>200000</v>
@@ -1171,7 +1175,7 @@
         <v>40000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>500000</v>
       </c>
@@ -1199,7 +1203,7 @@
         <v>250000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="3"/>
         <v>1000000</v>
@@ -1228,7 +1232,7 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="3"/>
         <v>2000000</v>
@@ -1257,7 +1261,7 @@
         <v>4000000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>5000000</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>25000000000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="3"/>
         <v>10000000</v>
@@ -1314,13 +1318,13 @@
         <v>100000000000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added charts to Week 4 spreadsheet
</commit_message>
<xml_diff>
--- a/Week4/KIT205_Week3.xlsx
+++ b/Week4/KIT205_Week3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/bronsonb_utas_edu_au/Documents/2025 - S1/KIT205/KIT205_575952/Week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="11_F7D9FA504A20DB2F5DD148760D251FD299863421" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4173CE1C-E306-4772-8C6C-CA244C66B0CD}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="11_F7D9FA504A20DB2F5DD148760D251FD299863421" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{409D4DF9-0E51-441A-8A47-C34346E82A33}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="683" windowWidth="14400" windowHeight="8182" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,8 +204,3455 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Function</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>T(f1)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4846</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T(f2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3403</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11575</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T(f3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>113</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T(f4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2895</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6554</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T(f5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$5:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>465</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T(f6)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$5:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3693</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11874</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T(f7)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$5:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-2524-480F-9F70-ECAEF94B2F73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2010825807"/>
+        <c:axId val="2010827727"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2010825807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2010827727"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2010827727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2010825807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Expected</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> times based on O()</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>g(n) = c log n</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$5:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3219280948873622</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3219280948873626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3219280948873626</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6438561897747244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6438561897747253</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6438561897747244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.287712379549451</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.287712379549451</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.287712379549449</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.609640474436812</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.609640474436812</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.609640474436812</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.931568569324174</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.931568569324174</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.931568569324174</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22.253496664211539</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.253496664211539</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1223-4149-8ED7-A0824FDC70A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g(n) = c n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1223-4149-8ED7-A0824FDC70A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g(n) = c n^2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$5:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2500000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10000000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40000000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>250000000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000000000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4000000000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25000000000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>100000000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1223-4149-8ED7-A0824FDC70A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2084065615"/>
+        <c:axId val="2084074255"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2084065615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2084074255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2084074255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2084065615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5EC0354-F25B-9768-65E4-FAEA751E6A1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>177331</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>560294</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>33616</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB878FB-D7C7-00CE-2D34-13FF385264E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,16 +3920,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="11" width="14.73046875" customWidth="1"/>
+    <col min="9" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
@@ -493,7 +3940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I3" s="3">
         <v>1</v>
       </c>
@@ -504,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +3989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -580,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>A5*2</f>
         <v>2</v>
@@ -619,7 +4066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -657,7 +4104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A26" si="3">A7*2</f>
         <v>10</v>
@@ -696,7 +4143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -735,7 +4182,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>50</v>
       </c>
@@ -773,7 +4220,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -812,7 +4259,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="3"/>
         <v>200</v>
@@ -851,7 +4298,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>500</v>
       </c>
@@ -889,7 +4336,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="3"/>
         <v>1000</v>
@@ -926,7 +4373,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="3"/>
         <v>2000</v>
@@ -963,7 +4410,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>5000</v>
       </c>
@@ -999,7 +4446,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="3"/>
         <v>10000</v>
@@ -1036,7 +4483,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="3"/>
         <v>20000</v>
@@ -1073,7 +4520,7 @@
         <v>400000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>50000</v>
       </c>
@@ -1109,7 +4556,7 @@
         <v>2500000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="3"/>
         <v>100000</v>
@@ -1144,7 +4591,7 @@
         <v>10000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="3"/>
         <v>200000</v>
@@ -1175,7 +4622,7 @@
         <v>40000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>500000</v>
       </c>
@@ -1203,7 +4650,7 @@
         <v>250000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="3"/>
         <v>1000000</v>
@@ -1232,7 +4679,7 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="3"/>
         <v>2000000</v>
@@ -1261,7 +4708,7 @@
         <v>4000000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>5000000</v>
       </c>
@@ -1289,7 +4736,7 @@
         <v>25000000000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="3"/>
         <v>10000000</v>
@@ -1318,17 +4765,18 @@
         <v>100000000000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>